<commit_message>
Mensaje que confirma los cambios
</commit_message>
<xml_diff>
--- a/Tamayo Obando Christian David Algoritmos y Pseudocódigo #2.xlsx
+++ b/Tamayo Obando Christian David Algoritmos y Pseudocódigo #2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\Primero Tics\Tamayo_ejercicio1\Tamayo_ejercicio1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\Primero Tics\Tamayo_Ejercicio1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B4F22A-5419-413A-BFA7-10BA03628FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A1E172-0F48-4D2E-8F7F-F1B698CBE07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,12 +111,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -148,26 +160,31 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE5E5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -444,272 +461,274 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3">
+      <c r="C7" s="4"/>
+      <c r="D7" s="1">
         <v>8.92</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>9.32</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <f>SUM(D7:F7)</f>
         <v>27.540000000000003</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <f>AVERAGE(D7:F7)</f>
         <v>9.1800000000000015</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3">
+      <c r="C8" s="4"/>
+      <c r="D8" s="1">
         <v>7.32</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>9.34</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>9.32</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <f t="shared" ref="G8:G14" si="0">SUM(D8:F8)</f>
         <v>25.98</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <f t="shared" ref="H8:H14" si="1">AVERAGE(D8:F8)</f>
         <v>8.66</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3">
+      <c r="C9" s="4"/>
+      <c r="D9" s="1">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>9.93</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>8.92</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
         <v>27.15</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <f t="shared" si="1"/>
         <v>9.0499999999999989</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3">
+      <c r="C10" s="4"/>
+      <c r="D10" s="1">
         <v>6.91</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>7.43</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
         <v>23.64</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <f t="shared" si="1"/>
         <v>7.88</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3">
+      <c r="C11" s="4"/>
+      <c r="D11" s="1">
         <v>9.4</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>9.5299999999999994</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <v>9.75</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>28.68</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <f t="shared" si="1"/>
         <v>9.56</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3">
+      <c r="C12" s="4"/>
+      <c r="D12" s="1">
         <v>7.9</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>9.4</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>7.3</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>24.6</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <f t="shared" si="1"/>
         <v>8.2000000000000011</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3">
+      <c r="C13" s="4"/>
+      <c r="D13" s="1">
         <v>8.92</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>8.34</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="1">
         <v>8.4499999999999993</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>25.709999999999997</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <f t="shared" si="1"/>
         <v>8.5699999999999985</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3">
+      <c r="C14" s="6"/>
+      <c r="D14" s="1">
         <v>9.32</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <v>9.32</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="1">
         <v>9.56</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>28.200000000000003</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <f t="shared" si="1"/>
         <v>9.4</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B2:I5"/>
     <mergeCell ref="H13:I13"/>
@@ -726,8 +745,6 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>